<commit_message>
added converting excel file entries to confession images
</commit_message>
<xml_diff>
--- a/src/files/test.xlsx
+++ b/src/files/test.xlsx
@@ -25,13 +25,13 @@
     <t>can we post this 👍</t>
   </si>
   <si>
-    <t>deez nuts</t>
+    <t>confession 1</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>your mother</t>
+    <t>confession 2</t>
   </si>
 </sst>
 </file>
@@ -39,19 +39,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -87,16 +81,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -412,12 +403,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="18.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +420,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>44848.42744212963</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -440,7 +431,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>44848.42791666667</v>
       </c>
       <c r="B3" s="2" t="s">

</xml_diff>